<commit_message>
Se realiza encoder 17 05 2024
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEGONZALEZ\Documents\Person\Maestria ciencia de datos\Machine Learning\Proyecto Obesidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F31FBF6-1575-4A5A-946C-4BCBD0314BF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23EDE85-9D4C-4F6C-B8A9-89E4D5633C0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12480" xr2:uid="{0FE59790-D139-4F6D-BCF6-01B27B4CF0B1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
   <si>
     <t>Variable Name</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Which transportation do you usually use?</t>
   </si>
   <si>
-    <t>NObeyesdad</t>
-  </si>
-  <si>
     <t>Target</t>
   </si>
   <si>
@@ -208,13 +205,28 @@
   </si>
   <si>
     <t>peso</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>Description2</t>
+  </si>
+  <si>
+    <t>OneHotEncoder</t>
+  </si>
+  <si>
+    <t>TargetEnconder</t>
+  </si>
+  <si>
+    <t>OrdinalEncoder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,13 +234,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -243,8 +267,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,22 +585,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5239D095-7D3A-4EF4-89A5-4A1CBE67A28B}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.28515625" customWidth="1"/>
-    <col min="6" max="6" width="75.140625" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="102.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="75.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,19 +612,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -607,17 +640,20 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -627,17 +663,17 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -647,14 +683,14 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -664,14 +700,14 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -681,17 +717,20 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -701,17 +740,20 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -721,17 +763,17 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -741,17 +783,17 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -761,17 +803,20 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
         <v>26</v>
       </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -781,17 +826,20 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -801,17 +849,17 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>30</v>
       </c>
-      <c r="F12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -821,17 +869,20 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -841,17 +892,17 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>34</v>
       </c>
-      <c r="F14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -861,17 +912,17 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>36</v>
       </c>
-      <c r="F15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -881,17 +932,20 @@
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="E16" t="s">
+      <c r="D16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
         <v>38</v>
       </c>
-      <c r="F16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -901,33 +955,39 @@
       <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="s">
-        <v>43</v>
+      <c r="D18" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>